<commit_message>
WIP: Add initial version of notas_fiscais.xlsx with ficha data
</commit_message>
<xml_diff>
--- a/notas_fiscais.xlsx
+++ b/notas_fiscais.xlsx
@@ -520,14 +520,10 @@
         </is>
       </c>
       <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>22/01/2026 20:35:58</t>
-        </is>
-      </c>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Erro ao pesquisar CPF</t>
+          <t>Erro ao selecionar atividade</t>
         </is>
       </c>
     </row>
@@ -568,14 +564,10 @@
         </is>
       </c>
       <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>22/01/2026 20:36:10</t>
-        </is>
-      </c>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Erro ao pesquisar CPF</t>
+          <t>Erro ao selecionar atividade</t>
         </is>
       </c>
     </row>
@@ -616,14 +608,10 @@
         </is>
       </c>
       <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>22/01/2026 20:36:22</t>
-        </is>
-      </c>
+      <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Erro ao pesquisar CPF</t>
+          <t>Erro ao selecionar atividade</t>
         </is>
       </c>
     </row>
@@ -664,14 +652,10 @@
         </is>
       </c>
       <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>22/01/2026 20:36:34</t>
-        </is>
-      </c>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Erro ao pesquisar CPF</t>
+          <t>Erro ao selecionar atividade</t>
         </is>
       </c>
     </row>

</xml_diff>